<commit_message>
Refactored code and Implemented adding worksheets
</commit_message>
<xml_diff>
--- a/test_excel1.xlsx
+++ b/test_excel1.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="12585"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId3" name="Sheet1" sheetId="1"/>
+    <sheet r:id="rId4" name="Sheet2" sheetId="2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -340,4 +341,16 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Option to add formules to sheet
</commit_message>
<xml_diff>
--- a/test_excel1.xlsx
+++ b/test_excel1.xlsx
@@ -360,6 +360,11 @@
         <v>120</v>
       </c>
     </row>
+    <row r="5">
+      <c r="D5" t="str">
+        <f>SUM(D2:D4)</f>
+      </c>
+    </row>
     <row r="7">
       <c r="E7" t="inlineStr">
         <is>

</xml_diff>